<commit_message>
Limpieza y Transformación de datos
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelalondonoocampo/Library/CloudStorage/GoogleDrive-mlondono.oc@gmail.com/Mi unidad/UDEA/LEA2-Analitica para la toma de decisiones/Ejercicios/T1-Aprendizaje Supervisado/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/alexander_bedoya1_udea_edu_co/Documents/Aprendizaje/Universidad/2023-2/Analítica II/Caso Estudio Supervisado/pediccion_abandono_empleo/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61313126-23D9-45CE-8B5F-37C1DF73E553}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diccionario" sheetId="1" r:id="rId1"/>
+    <sheet name="general_data" sheetId="1" r:id="rId1"/>
+    <sheet name="employee_survey_data" sheetId="2" r:id="rId2"/>
+    <sheet name="manager_survey_data" sheetId="3" r:id="rId3"/>
+    <sheet name="time_work" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Age</t>
   </si>
@@ -46,9 +62,6 @@
     <t>EmployeeCount</t>
   </si>
   <si>
-    <t>EmployeeNumber</t>
-  </si>
-  <si>
     <t>EnvironmentSatisfaction</t>
   </si>
   <si>
@@ -263,6 +276,9 @@
   </si>
   <si>
     <t>Tiempo promedio de trabajo al día del empleado en el ultimo año</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
   </si>
 </sst>
 </file>
@@ -405,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,6 +604,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,18 +826,39 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -882,6 +925,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,487 +1228,618 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="2" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="2" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="7"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="8"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C54" s="2"/>
+      <c r="C33" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A26:A29"/>
+  <mergeCells count="4">
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2818FF91-424B-41C1-B6E0-67943892BAFF}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB347B72-1368-4B4D-BDDB-3022C8711B7B}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A7:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F96770A-4BBC-4F98-BC74-C0490B824320}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tablas y visualizaciones EDA variables categóricas.
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61313126-23D9-45CE-8B5F-37C1DF73E553}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1740" yWindow="1740" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_data" sheetId="1" r:id="rId1"/>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1546,7 +1546,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="B11" sqref="B11:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB347B72-1368-4B4D-BDDB-3022C8711B7B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Análisis de correlación de variables numéricas independientes
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61313126-23D9-45CE-8B5F-37C1DF73E553}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1740" yWindow="1740" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_data" sheetId="1" r:id="rId1"/>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB347B72-1368-4B4D-BDDB-3022C8711B7B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Preparación de los datos.
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/alexander_bedoya1_udea_edu_co/Documents/Aprendizaje/Universidad/2023-2/Analítica II/Caso Estudio Supervisado/pediccion_abandono_empleo/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61313126-23D9-45CE-8B5F-37C1DF73E553}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3980A92F-747C-49CE-A9B7-79BDB973517C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +610,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -826,7 +832,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -868,6 +874,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1230,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,31 +1280,31 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1298,61 +1316,61 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -1364,40 +1382,40 @@
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="16"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -1690,7 +1708,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Separando funciones en utils.py
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/alexander_bedoya1_udea_edu_co/Documents/Aprendizaje/Universidad/2023-2/Analítica II/Caso Estudio Supervisado/pediccion_abandono_empleo/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3980A92F-747C-49CE-A9B7-79BDB973517C}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607CFC27-01B9-4868-96FC-F71278066353}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>Age</t>
   </si>
@@ -98,9 +98,6 @@
     <t>PerformanceRating</t>
   </si>
   <si>
-    <t>RelationshipSatisfaction</t>
-  </si>
-  <si>
     <t>StandardHours</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Valoración del rendimiento en el último año</t>
   </si>
   <si>
-    <t>Nivel de satisfacción de la relación</t>
-  </si>
-  <si>
     <t>Horas estándar de trabajo del empleado</t>
   </si>
   <si>
@@ -272,13 +266,16 @@
     <t>Nivel (Categóricas)</t>
   </si>
   <si>
-    <t>mean_work</t>
-  </si>
-  <si>
     <t>Tiempo promedio de trabajo al día del empleado en el ultimo año</t>
   </si>
   <si>
     <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>mean_time</t>
+  </si>
+  <si>
+    <t>Descripción</t>
   </si>
 </sst>
 </file>
@@ -421,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,18 +601,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +817,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -844,18 +829,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -875,16 +848,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1246,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,13 +1234,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1275,154 +1248,154 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="16"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="16"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="16"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="17" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="16" t="s">
+      <c r="C12" s="12"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="16"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="16"/>
+      <c r="B15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="16"/>
+      <c r="B18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="4"/>
     </row>
@@ -1431,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4"/>
     </row>
@@ -1440,7 +1413,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -1449,111 +1422,195 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="A25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="A26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="4"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="11"/>
+      <c r="B45" s="8"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B23:B26"/>
+  <mergeCells count="12">
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1564,7 +1621,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B14"/>
+      <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,118 +1633,118 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>41</v>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>52</v>
+      <c r="A11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="2" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1765,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B10"/>
+      <selection activeCell="A3" sqref="A3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,86 +1777,86 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1875,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1830,21 +1887,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1853,7 +1910,7 @@
         <v>78</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4"/>
     </row>

</xml_diff>

<commit_message>
Inicio de preparación de datos (Valores atípicos).
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607CFC27-01B9-4868-96FC-F71278066353}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_data" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -831,15 +831,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -848,16 +839,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1221,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,142 +1241,142 @@
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="12" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -1490,104 +1478,104 @@
       <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="7"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="10"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="10"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="8"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="10"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="10"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="10"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="11"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="7"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="8"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="11"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
@@ -1599,6 +1587,10 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A46:A49"/>
     <mergeCell ref="B46:B49"/>
     <mergeCell ref="A34:A37"/>
@@ -1607,10 +1599,6 @@
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1652,10 +1640,10 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1663,31 +1651,31 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1695,31 +1683,31 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1727,22 +1715,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
@@ -1796,10 +1784,10 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1807,31 +1795,31 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1839,22 +1827,22 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Terminando conclusiones de análisis univariado de categóricas.
</commit_message>
<xml_diff>
--- a/Datasets/data_dictionary.xlsx
+++ b/Datasets/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/alexander_bedoya1_udea_edu_co/Documents/Aprendizaje/Universidad/2023-2/Analítica II/Caso Estudio Supervisado/pediccion_abandono_empleo/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{607CFC27-01B9-4868-96FC-F71278066353}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{A714B8F1-2F1C-BA45-AC45-04952E0FE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B496AC5-FCFB-4610-AC2E-D316EB9F1618}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Age</t>
   </si>
@@ -831,6 +831,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -838,15 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1207,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1277,10 +1277,10 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1288,29 +1288,29 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
         <v>59</v>
       </c>
@@ -1477,128 +1477,10 @@
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="10"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="11"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="11"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="10"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="10"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="10"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="11"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="10"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="10"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="11"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="2">
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1640,10 +1522,10 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1651,31 +1533,31 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1683,31 +1565,31 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1715,22 +1597,22 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
@@ -1752,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB347B72-1368-4B4D-BDDB-3022C8711B7B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B10"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,10 +1666,10 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1795,31 +1677,31 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1827,22 +1709,22 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
         <v>68</v>
       </c>

</xml_diff>